<commit_message>
purchase page test cases executed
</commit_message>
<xml_diff>
--- a/exec/symlex_vpn_ windows/test_cases(app)/report_summary.xlsx
+++ b/exec/symlex_vpn_ windows/test_cases(app)/report_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\office\SymlexVPNTestCases\exec\symlex_vpn_ windows\test_cases(app)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\exec\symlex_vpn_ windows\test_cases(app)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9302C927-5537-42EA-B6A0-A6BD6EEDCDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF6A7D4-0C46-400B-8E68-D809AC448764}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="6" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="features" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="53">
   <si>
     <t>Features of enter vpn</t>
   </si>
@@ -130,80 +130,90 @@
   </si>
   <si>
     <t>SYMREDVOU-022</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (15-02-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_STP_021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (19-02-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (20-02-24)</t>
+  </si>
+  <si>
+    <t>SYM-WIN-LOG-029</t>
+  </si>
+  <si>
+    <t>TC_SYM_MA_006,
+TC_SYM_MA_023,
+TC_SYM_MA_024</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (22-02-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (26-02-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_AC_011,
+TC_SYM_AC_012,
+TC_SYM_AC_013</t>
+  </si>
+  <si>
+    <t>SYMFREEBON-074,
+SYMFREEBON-075,
+SYMFREEBON-076</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (04-03-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (06-03-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_GSF_0021</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (07-03-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (10-03-24)</t>
+  </si>
+  <si>
+    <t>TC_SYM_SP_017,
+TC_SYM_SP_029,
+TC_SYM_SP_030</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (11-03-24)</t>
+  </si>
+  <si>
+    <t>SYMREDVOU-022,
+SYMREDVOU-023</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (12-03-24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case Summary (27-03-24)</t>
   </si>
   <si>
     <t>SYM-PP-04,
 SYM-PP-08,
 SYM-PP-019,
-SYM-PP-022,
-SYM-PP-024,
-SYM-PP-025</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (15-02-24)</t>
-  </si>
-  <si>
-    <t>TC_SYM_STP_021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (19-02-24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (20-02-24)</t>
-  </si>
-  <si>
-    <t>SYM-WIN-LOG-029</t>
-  </si>
-  <si>
-    <t>TC_SYM_MA_006,
-TC_SYM_MA_023,
-TC_SYM_MA_024</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (22-02-24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (26-02-24)</t>
-  </si>
-  <si>
-    <t>TC_SYM_AC_011,
-TC_SYM_AC_012,
-TC_SYM_AC_013</t>
-  </si>
-  <si>
-    <t>SYMFREEBON-074,
-SYMFREEBON-075,
-SYMFREEBON-076</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (04-03-24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (06-03-24)</t>
-  </si>
-  <si>
-    <t>TC_SYM_GSF_0021</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (07-03-24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (10-03-24)</t>
-  </si>
-  <si>
-    <t>TC_SYM_SP_017,
-TC_SYM_SP_029,
-TC_SYM_SP_030</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (11-03-24)</t>
-  </si>
-  <si>
-    <t>SYMREDVOU-022,
-SYMREDVOU-023</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Test Case Summary (12-03-24)</t>
+SYM-PP-026,
+SYM-PP-027,
+SYM-PP-028</t>
+  </si>
+  <si>
+    <t>SYM-PP-04,
+SYM-PP-08,
+SYM-PP-019,
+SYM-PP-026,
+SYM-PP-027</t>
   </si>
 </sst>
 </file>
@@ -691,9 +701,9 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="32.140625" customWidth="1"/>
+    <col min="2" max="2" width="32.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:2" ht="21">
@@ -800,24 +810,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D112B8-BA61-4323-A81E-60AEE54129B4}">
   <dimension ref="D2:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -825,7 +835,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -833,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -841,7 +851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -857,13 +867,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="4:5" ht="18.75">
+    <row r="11" spans="4:5" ht="18">
       <c r="D11" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E11" s="14"/>
     </row>
-    <row r="12" spans="4:5" ht="18.75">
+    <row r="12" spans="4:5" ht="18">
       <c r="D12" s="1" t="s">
         <v>20</v>
       </c>
@@ -871,7 +881,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="4:5" ht="18.75">
+    <row r="13" spans="4:5" ht="18">
       <c r="D13" s="3" t="s">
         <v>21</v>
       </c>
@@ -879,7 +889,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="4:5" ht="18.75">
+    <row r="14" spans="4:5" ht="18">
       <c r="D14" s="2" t="s">
         <v>22</v>
       </c>
@@ -887,7 +897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="4:5" ht="18.75">
+    <row r="15" spans="4:5" ht="18">
       <c r="D15" s="5" t="s">
         <v>23</v>
       </c>
@@ -900,7 +910,7 @@
         <v>24</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -920,20 +930,20 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -941,7 +951,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -949,7 +959,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -957,7 +967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -987,20 +997,20 @@
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1008,7 +1018,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1016,7 +1026,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1024,7 +1034,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1037,7 +1047,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1056,20 +1066,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1077,7 +1087,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1095,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1093,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1106,7 +1116,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1125,20 +1135,20 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1146,7 +1156,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1154,7 +1164,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1162,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1192,20 +1202,20 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1213,7 +1223,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1221,7 +1231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1229,7 +1239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1259,20 +1269,20 @@
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1280,7 +1290,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1296,7 +1306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1326,20 +1336,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1347,7 +1357,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1355,7 +1365,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1363,7 +1373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1395,19 +1405,19 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="29.85546875" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:7" ht="18.75">
+    <row r="2" spans="3:7" ht="18">
       <c r="C2" s="13" t="s">
         <v>27</v>
       </c>
       <c r="D2" s="14"/>
     </row>
-    <row r="3" spans="3:7" ht="18.75">
+    <row r="3" spans="3:7" ht="18">
       <c r="C3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1415,7 +1425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="3:7" ht="18.75">
+    <row r="4" spans="3:7" ht="18">
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1423,7 +1433,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="3:7" ht="18.75">
+    <row r="5" spans="3:7" ht="18">
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1432,7 +1442,7 @@
       </c>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="3:7" ht="18.75">
+    <row r="6" spans="3:7" ht="18">
       <c r="C6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1465,20 +1475,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1486,7 +1496,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1494,7 +1504,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1502,7 +1512,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1515,7 +1525,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1534,20 +1544,20 @@
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1555,7 +1565,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1563,7 +1573,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1571,7 +1581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1601,20 +1611,20 @@
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1622,7 +1632,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1630,7 +1640,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1638,7 +1648,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1670,20 +1680,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1691,7 +1701,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1699,7 +1709,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1707,7 +1717,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1720,7 +1730,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1739,20 +1749,20 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1760,7 +1770,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1768,7 +1778,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1776,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1806,20 +1816,20 @@
       <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1827,7 +1837,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1835,7 +1845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1843,7 +1853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1856,7 +1866,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1875,20 +1885,20 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
         <v>19</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1896,7 +1906,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
@@ -1904,7 +1914,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="4:5" ht="18.75">
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
@@ -1912,7 +1922,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:5" ht="18.75">
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>24</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -1938,26 +1948,26 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20E9BD1-861C-4DAA-A578-3640159897E0}">
-  <dimension ref="D2:E8"/>
+  <dimension ref="D2:E17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
-    <col min="3" max="3" width="3.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="3.5546875" customWidth="1"/>
+    <col min="4" max="4" width="37.109375" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:5" ht="18.75">
+    <row r="2" spans="4:5" ht="18">
       <c r="D2" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E2" s="14"/>
     </row>
-    <row r="3" spans="4:5" ht="18.75">
+    <row r="3" spans="4:5" ht="18">
       <c r="D3" s="1" t="s">
         <v>20</v>
       </c>
@@ -1965,23 +1975,23 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="4:5" ht="18.75">
+    <row r="4" spans="4:5" ht="18">
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E4" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="4:5" ht="18.75">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" ht="18">
       <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="E5" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="4:5" ht="18.75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="18">
       <c r="D6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1994,12 +2004,59 @@
         <v>24</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="18">
+      <c r="D11" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E11" s="14"/>
+    </row>
+    <row r="12" spans="4:5" ht="18">
+      <c r="D12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="18">
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" ht="18">
+      <c r="D14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="18">
+      <c r="D15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="4:5" ht="102" customHeight="1">
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>